<commit_message>
change from X1 to J
</commit_message>
<xml_diff>
--- a/data/Dataset_MODAN_initial.xlsx
+++ b/data/Dataset_MODAN_initial.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpro13-6/Desktop/MODAN/抗菌ペプチド/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD12B4F-ED70-EB4B-96E8-5008EE86D0E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C1C944E-13AE-2F47-AEED-88C1D76AB018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{25C599C3-B986-5743-8D39-AC0174F00E63}"/>
   </bookViews>
@@ -709,10 +709,6 @@
     <t>[H]NCC(N[C@]([C@@H](C)CC)([H])C(N[C@@H](CCN)C(N[C@@H](CCN)C(N[C@H](C(N[C@@H](CC(C)C)C(N[C@@H](CCN)C(N[C@@H](CO)C(NC(C(N[C@@H](CCN)C(N[C@@H](CCN)C(N[C@H](C(N[C@@H](C(C)C)C(N[C@@H](CCN)C(NC(C(N[C@H](C(N[C@@H](CCN)C(N)=O)=O)CC1=CC=CC=C1)=O)(C)C)=O)=O)=O)CC2=CC=CC=C2)=O)=O)=O)(C)C)=O)=O)=O)=O)CC3=CC=CC=C3)=O)=O)=O)=O</t>
   </si>
   <si>
-    <t>H-GIX1X1FLX1SUX1X1FVX1UFX1-NH2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>H-GIRRFLRSURRFVRUFR-NH2</t>
   </si>
   <si>
@@ -748,15 +744,7 @@
     <t>[H]NCC(N[C@]([C@@H](C)CC)([H])C(N[C@@H](CCCCN)C(N[C@@H](CCN)C(N[C@H](C(N[C@@H](CC(C)C)C(N[C@@H](CCCCN)C(N[C@@H](CO)C(NC(C(N[C@@H](CCN)C(N[C@@H](CCCCN)C(N[C@H](C(N[C@@H](C(C)C)C(N[C@@H](CCN)C(NC(C(N[C@H](C(N[C@@H](CCCCN)C(N)=O)=O)CC1=CC=CC=C1)=O)(C)C)=O)=O)=O)CC2=CC=CC=C2)=O)=O)=O)(C)C)=O)=O)=O)=O)CC3=CC=CC=C3)=O)=O)=O)=O</t>
   </si>
   <si>
-    <t>H-GIKX1FLKSUX1KFVX1UFK-NH2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>[H]NCC(N[C@]([C@@H](C)CC)([H])C(N[C@@H](CCN)C(N[C@@H](CCCCN)C(N[C@H](C(N[C@@H](CC(C)C)C(N[C@@H](CCN)C(N[C@@H](CO)C(NC(C(N[C@@H](CCCCN)C(N[C@@H](CCN)C(N[C@H](C(N[C@@H](C(C)C)C(N[C@@H](CCCCN)C(NC(C(N[C@H](C(N[C@@H](CCN)C(N)=O)=O)CC1=CC=CC=C1)=O)(C)C)=O)=O)=O)CC2=CC=CC=C2)=O)=O)=O)(C)C)=O)=O)=O)=O)CC3=CC=CC=C3)=O)=O)=O)=O</t>
-  </si>
-  <si>
-    <t>H-GIX1KFLX1SUKX1FVKUFX1-NH2</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>H-GIKRFLKSURKFVRUFK-NH2</t>
@@ -812,15 +800,7 @@
     <t>[H]NCC(N[C@]([C@@H](C)CC)([H])C(N[C@@H](CCCCN)C(N[C@@H](CCCCN)C(N[C@H](C(N[C@@H](CC(C)C)C(N[C@@H](CCCCN)C(N[C@@H](CO)C(NC(C(N[C@@H](CCN)C(N[C@@H](CCN)C(N[C@H](C(N[C@@H](C(C)C)C(N[C@@H](CCN)C(NC(C(N[C@H](C(N[C@@H](CCN)C(N)=O)=O)CC1=CC=CC=C1)=O)(C)C)=O)=O)=O)CC2=CC=CC=C2)=O)=O)=O)(C)C)=O)=O)=O)=O)CC3=CC=CC=C3)=O)=O)=O)=O</t>
   </si>
   <si>
-    <t>H-GIKKFLKSUX1X1FVX1UFX1-NH2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>[H]NCC(N[C@]([C@@H](C)CC)([H])C(N[C@@H](CCN)C(N[C@@H](CCN)C(N[C@H](C(N[C@@H](CC(C)C)C(N[C@@H](CCN)C(N[C@@H](CO)C(NC(C(N[C@@H](CCCCN)C(N[C@@H](CCCCN)C(N[C@H](C(N[C@@H](C(C)C)C(N[C@@H](CCCCN)C(NC(C(N[C@H](C(N[C@@H](CCCCN)C(N)=O)=O)CC1=CC=CC=C1)=O)(C)C)=O)=O)=O)CC2=CC=CC=C2)=O)=O)=O)(C)C)=O)=O)=O)=O)CC3=CC=CC=C3)=O)=O)=O)=O</t>
-  </si>
-  <si>
-    <t>H-GIX1X1FLX1SUKKFVKUFK-NH2</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>H-GIKKFLKSURRFVRUFR-NH2</t>
@@ -1204,6 +1184,26 @@
   </si>
   <si>
     <t>Hemolysis</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>H-GIJJFLJSUJJFVJUFJ-NH2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>H-GIKJFLKSUJKFVJUFK-NH2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>H-GIJKFLJSUKJFVKUFJ-NH2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>H-GIKKFLKSUJJFVJUFJ-NH2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>H-GIJJFLJSUKKFVKUFK-NH2</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1734,8 +1734,8 @@
   </sheetPr>
   <dimension ref="A1:K90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+    <sheetView tabSelected="1" topLeftCell="F61" zoomScale="164" zoomScaleNormal="59" workbookViewId="0">
+      <selection activeCell="J63" sqref="J63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="20"/>
@@ -1759,28 +1759,28 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="105">
@@ -2042,7 +2042,7 @@
         <v>12.5</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="J10" t="s">
         <v>21</v>
@@ -2930,7 +2930,7 @@
         <v>25</v>
       </c>
       <c r="J46" t="s">
-        <v>97</v>
+        <v>174</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="126">
@@ -2939,7 +2939,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D47" s="1">
         <v>3.125</v>
@@ -2957,7 +2957,7 @@
         <v>6.25</v>
       </c>
       <c r="J47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="126">
@@ -2966,7 +2966,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>89</v>
@@ -2984,7 +2984,7 @@
         <v>5</v>
       </c>
       <c r="J48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="147">
@@ -2993,7 +2993,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>89</v>
@@ -3005,7 +3005,7 @@
         <v>5</v>
       </c>
       <c r="J49" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="105">
@@ -3014,7 +3014,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D50" s="1">
         <v>1.56</v>
@@ -3032,7 +3032,7 @@
         <v>50</v>
       </c>
       <c r="J50" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="105">
@@ -3041,7 +3041,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D51" s="1">
         <v>1.56</v>
@@ -3059,7 +3059,7 @@
         <v>100</v>
       </c>
       <c r="J51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="105">
@@ -3068,7 +3068,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D52" s="1">
         <v>1.56</v>
@@ -3086,7 +3086,7 @@
         <v>50</v>
       </c>
       <c r="J52" t="s">
-        <v>109</v>
+        <v>175</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="105">
@@ -3095,7 +3095,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D53" s="1">
         <v>1.56</v>
@@ -3113,7 +3113,7 @@
         <v>50</v>
       </c>
       <c r="J53" t="s">
-        <v>111</v>
+        <v>176</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="105">
@@ -3122,7 +3122,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D54" s="1">
         <v>1.56</v>
@@ -3140,7 +3140,7 @@
         <v>25</v>
       </c>
       <c r="J54" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="105">
@@ -3149,7 +3149,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D55" s="1">
         <v>3.125</v>
@@ -3167,7 +3167,7 @@
         <v>25</v>
       </c>
       <c r="J55" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="105">
@@ -3176,7 +3176,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D56" s="1">
         <v>6.25</v>
@@ -3194,7 +3194,7 @@
         <v>5</v>
       </c>
       <c r="J56" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="105">
@@ -3203,7 +3203,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D57" s="1">
         <v>6.25</v>
@@ -3221,7 +3221,7 @@
         <v>5</v>
       </c>
       <c r="J57" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="105">
@@ -3230,7 +3230,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>89</v>
@@ -3248,7 +3248,7 @@
         <v>0.78</v>
       </c>
       <c r="J58" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="126">
@@ -3257,7 +3257,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>89</v>
@@ -3275,7 +3275,7 @@
         <v>0.78</v>
       </c>
       <c r="J59" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="105">
@@ -3284,7 +3284,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D60" s="1">
         <v>1.56</v>
@@ -3302,7 +3302,7 @@
         <v>50</v>
       </c>
       <c r="J60" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="105">
@@ -3311,7 +3311,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D61" s="1">
         <v>1.56</v>
@@ -3329,7 +3329,7 @@
         <v>50</v>
       </c>
       <c r="J61" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="105">
@@ -3338,7 +3338,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D62" s="1">
         <v>1.56</v>
@@ -3356,7 +3356,7 @@
         <v>50</v>
       </c>
       <c r="J62" t="s">
-        <v>129</v>
+        <v>177</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="105">
@@ -3365,7 +3365,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D63" s="1">
         <v>1.56</v>
@@ -3383,7 +3383,7 @@
         <v>12.5</v>
       </c>
       <c r="J63" t="s">
-        <v>131</v>
+        <v>178</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="105">
@@ -3392,7 +3392,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D64" s="1">
         <v>1.56</v>
@@ -3410,7 +3410,7 @@
         <v>50</v>
       </c>
       <c r="J64" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="105">
@@ -3419,7 +3419,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D65" s="1">
         <v>1.56</v>
@@ -3437,16 +3437,16 @@
         <v>25</v>
       </c>
       <c r="J65" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="105">
       <c r="A66">
-        <f t="shared" ref="A66:A84" si="1">ROW()-1</f>
+        <f t="shared" ref="A66:A83" si="1">ROW()-1</f>
         <v>65</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D66" s="1">
         <v>6.25</v>
@@ -3464,7 +3464,7 @@
         <v>5</v>
       </c>
       <c r="J66" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="105">
@@ -3473,7 +3473,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D67" s="1">
         <v>6.25</v>
@@ -3491,7 +3491,7 @@
         <v>5</v>
       </c>
       <c r="J67" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="126">
@@ -3500,7 +3500,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>89</v>
@@ -3518,7 +3518,7 @@
         <v>0.19</v>
       </c>
       <c r="J68" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="126">
@@ -3527,7 +3527,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D69" s="1">
         <v>50</v>
@@ -3545,7 +3545,7 @@
         <v>0.78</v>
       </c>
       <c r="J69" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="105">
@@ -3554,7 +3554,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C70" s="1">
         <v>3.125</v>
@@ -3575,7 +3575,7 @@
         <v>5</v>
       </c>
       <c r="J70" s="6" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="105">
@@ -3584,7 +3584,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D71" s="1">
         <v>12.5</v>
@@ -3602,7 +3602,7 @@
         <v>5</v>
       </c>
       <c r="J71" s="6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="105">
@@ -3611,7 +3611,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D72" s="1">
         <v>1.56</v>
@@ -3629,7 +3629,7 @@
         <v>5</v>
       </c>
       <c r="J72" s="6" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="105">
@@ -3638,7 +3638,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D73" s="1">
         <v>3.125</v>
@@ -3656,7 +3656,7 @@
         <v>1.56</v>
       </c>
       <c r="J73" s="6" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="105">
@@ -3665,7 +3665,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D74" s="1">
         <v>6.25</v>
@@ -3683,7 +3683,7 @@
         <v>0.78</v>
       </c>
       <c r="J74" s="6" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="126">
@@ -3692,7 +3692,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D75" s="1">
         <v>6.25</v>
@@ -3710,7 +3710,7 @@
         <v>1.56</v>
       </c>
       <c r="J75" s="6" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="105">
@@ -3719,7 +3719,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D76" s="1">
         <v>1.56</v>
@@ -3737,7 +3737,7 @@
         <v>12.5</v>
       </c>
       <c r="J76" s="6" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="105">
@@ -3746,7 +3746,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D77" s="1">
         <v>6.25</v>
@@ -3764,7 +3764,7 @@
         <v>0.78</v>
       </c>
       <c r="J77" s="6" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="105">
@@ -3773,7 +3773,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>89</v>
@@ -3791,7 +3791,7 @@
         <v>0.78</v>
       </c>
       <c r="J78" s="6" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="105">
@@ -3800,7 +3800,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>5</v>
@@ -3821,7 +3821,7 @@
         <v>5</v>
       </c>
       <c r="J79" s="6" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="105">
@@ -3830,7 +3830,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>5</v>
@@ -3851,7 +3851,7 @@
         <v>5</v>
       </c>
       <c r="J80" s="6" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="105">
@@ -3860,7 +3860,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>5</v>
@@ -3881,7 +3881,7 @@
         <v>5</v>
       </c>
       <c r="J81" s="6" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="105">
@@ -3890,7 +3890,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>5</v>
@@ -3911,7 +3911,7 @@
         <v>5</v>
       </c>
       <c r="J82" s="6" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="84">
@@ -3920,7 +3920,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>5</v>
@@ -3941,7 +3941,7 @@
         <v>5</v>
       </c>
       <c r="J83" s="6" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="84" spans="1:10">

</xml_diff>